<commit_message>
06-24-23 08:18 [Added auto refresh and lastID]
</commit_message>
<xml_diff>
--- a/GUI/registration/employees.xlsx
+++ b/GUI/registration/employees.xlsx
@@ -466,7 +466,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1212</t>
+          <t>EMP_1</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -476,7 +476,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>sample@yahoocheese.com</t>
+          <t>ryann@mail.com</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -486,81 +486,81 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Ewam</t>
+          <t>BSIT</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>091234567890</t>
+          <t>09123456789</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>1k</t>
+          <t>1000</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Sample</t>
+          <t>Sa bahay</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>123</t>
+          <t>EMP_2</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>sdfdh</t>
+          <t>Malabanan, RySes</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>oihoi</t>
+          <t>ryses@email.com</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>hoih</t>
+          <t>male</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>oiiho</t>
+          <t>BSIT</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>hooih</t>
+          <t>09123456789</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>iuho</t>
+          <t>160</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>ihopih</t>
+          <t>Sa bahay</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>sample</t>
+          <t>EMP_3</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Malabanan, RySes</t>
+          <t>Malabanan, Kim</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>ryses@developer.com</t>
+          <t>kim@email.com</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -570,7 +570,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>IT Dept</t>
+          <t>BSIT</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -580,12 +580,12 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>1000</t>
+          <t>100</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>charot</t>
+          <t>Sample</t>
         </is>
       </c>
     </row>

</xml_diff>